<commit_message>
glava 4 i 5
</commit_message>
<xml_diff>
--- a/Rezultati/Rezultati.xlsx
+++ b/Rezultati/Rezultati.xlsx
@@ -449,8 +449,8 @@
   </sheetPr>
   <dimension ref="A1:P284"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A113" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S143" activeCellId="0" sqref="S143"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A116" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N126" activeCellId="0" sqref="N126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>